<commit_message>
consolidated all to one sheet
</commit_message>
<xml_diff>
--- a/REVER_DailyTracker_20200928.xlsx
+++ b/REVER_DailyTracker_20200928.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Monisha\Desktop\Daily_Tracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mamatha\DailyTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6803AFB0-1FF7-4470-8D3F-852FA2CC9C6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F465E71-B080-494E-BC0F-AA9829771919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Balraj" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="171">
   <si>
     <t>No</t>
   </si>
@@ -448,20 +448,136 @@
   <si>
     <t>2020-09028</t>
   </si>
+  <si>
+    <t>QMVAr-RPA</t>
+  </si>
+  <si>
+    <t>Purchase Summary issue on date</t>
+  </si>
+  <si>
+    <t>Corrected the date logic and tested</t>
+  </si>
+  <si>
+    <t>Hayaai-B2B</t>
+  </si>
+  <si>
+    <t>Working on B2B stored procedure in creating the company</t>
+  </si>
+  <si>
+    <t>Service Request -B2B issue tracker issues resolving</t>
+  </si>
+  <si>
+    <t>Sony-QMVAR</t>
+  </si>
+  <si>
+    <t>RMS MVS upload testing</t>
+  </si>
+  <si>
+    <t>RMS Invoice captcha integration with GOOGLE API</t>
+  </si>
+  <si>
+    <t>QMVAR-PR summary five days</t>
+  </si>
+  <si>
+    <t>Rahman San had given this task for credit info,had completed</t>
+  </si>
+  <si>
+    <t>Trying to resolve B2B issues from issue tracke</t>
+  </si>
+  <si>
+    <t>Trying to complete issues from issue tracker</t>
+  </si>
+  <si>
+    <t>QMVAR-Sony</t>
+  </si>
+  <si>
+    <t>RMS invoice captcha issues,relogin with recaptcha,error msg for 20 mins</t>
+  </si>
+  <si>
+    <t>Given code to Mohan sir</t>
+  </si>
+  <si>
+    <t>B2B-New api for product type addition</t>
+  </si>
+  <si>
+    <t>Product category api,IMEI check new API are developed</t>
+  </si>
+  <si>
+    <t>B2B issues from issue tracker</t>
+  </si>
+  <si>
+    <t>HAYAAI-B2B</t>
+  </si>
+  <si>
+    <t>Reports corrections and signup corrections</t>
+  </si>
+  <si>
+    <t>signup corrections and table corrections</t>
+  </si>
+  <si>
+    <t>Search errors in Service Request and Jib correction</t>
+  </si>
+  <si>
+    <t>HAYAAI-B2C</t>
+  </si>
+  <si>
+    <t>Issue description passing to Jobs failure</t>
+  </si>
+  <si>
+    <t>HAYAAI-B2B and B2C</t>
+  </si>
+  <si>
+    <t>Few corrections in B2B APP and flow on Pick Delivery change for B2C reviewing</t>
+  </si>
+  <si>
+    <t>DRS Count - Saw Discount with out discount</t>
+  </si>
+  <si>
+    <t>Warranty Status to be saved in Add Devices</t>
+  </si>
+  <si>
+    <t>Pickup delivery new update customer info passing to Job</t>
+  </si>
+  <si>
+    <t>New Push Notification while technician starting for Job</t>
+  </si>
+  <si>
+    <t>HAYAAI-QMVAR</t>
+  </si>
+  <si>
+    <t>B2B- Testing</t>
+  </si>
+  <si>
+    <t>New functionality adding new API for technician tracking</t>
+  </si>
+  <si>
+    <t>Pickup time correction as it was not stored correctly</t>
+  </si>
+  <si>
+    <t>Issue corrections from issue tracker</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-14009]yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="[$-14009]mm/dd/yyyy;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -523,7 +639,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -563,6 +679,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,15 +803,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -697,12 +819,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -729,7 +851,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -738,16 +860,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -756,14 +878,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -776,12 +898,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -795,24 +917,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -846,6 +950,51 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2558,19 +2707,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="6.109375" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" style="79" customWidth="1"/>
     <col min="6" max="6" width="18.109375" customWidth="1"/>
     <col min="7" max="7" width="48.6640625" customWidth="1"/>
   </cols>
@@ -2588,7 +2737,7 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="76" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -2599,71 +2748,474 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="4"/>
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="72">
+        <v>44075</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="77">
+        <v>1</v>
+      </c>
+      <c r="F2" s="83" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="8"/>
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="72">
+        <v>44076</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="77">
+        <v>0.8</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1"/>
-    <row r="5" spans="1:7" s="1" customFormat="1"/>
-    <row r="6" spans="1:7" s="1" customFormat="1"/>
-    <row r="7" spans="1:7" s="1" customFormat="1"/>
-    <row r="8" spans="1:7" s="1" customFormat="1"/>
-    <row r="9" spans="1:7" s="1" customFormat="1"/>
-    <row r="10" spans="1:7" s="1" customFormat="1"/>
-    <row r="11" spans="1:7" s="1" customFormat="1"/>
-    <row r="12" spans="1:7" s="1" customFormat="1"/>
-    <row r="13" spans="1:7" s="1" customFormat="1"/>
-    <row r="14" spans="1:7" s="1" customFormat="1"/>
-    <row r="15" spans="1:7" s="1" customFormat="1"/>
-    <row r="16" spans="1:7" s="1" customFormat="1"/>
-    <row r="17" spans="2:3" s="1" customFormat="1"/>
-    <row r="18" spans="2:3" s="1" customFormat="1"/>
-    <row r="19" spans="2:3" s="1" customFormat="1"/>
-    <row r="22" spans="2:3">
-      <c r="C22" s="9" t="s">
+    <row r="4" spans="1:7" s="1" customFormat="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="73">
+        <v>44077</v>
+      </c>
+      <c r="C4" s="84" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="78">
+        <v>0.4</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1">
+      <c r="A5" s="86">
+        <v>4</v>
+      </c>
+      <c r="B5" s="73">
+        <v>44078</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="78">
+        <v>0.8</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1">
+      <c r="A6" s="86">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="B23" s="10"/>
+      <c r="B6" s="73">
+        <v>44081</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="78">
+        <v>0.6</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1">
+      <c r="A7" s="86">
+        <v>6</v>
+      </c>
+      <c r="B7" s="73">
+        <v>44082</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7" s="78">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1">
+      <c r="A8" s="86">
+        <v>7</v>
+      </c>
+      <c r="B8" s="73">
+        <v>44083</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E8" s="78">
+        <v>0.4</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1">
+      <c r="A9" s="86">
+        <v>8</v>
+      </c>
+      <c r="B9" s="73">
+        <v>44084</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="78">
+        <v>0.6</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1">
+      <c r="A10" s="86">
+        <v>9</v>
+      </c>
+      <c r="B10" s="73">
+        <v>44085</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E10" s="78">
+        <v>0.8</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1">
+      <c r="A11" s="86">
+        <v>10</v>
+      </c>
+      <c r="B11" s="73">
+        <v>44088</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="78">
+        <v>0.6</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1">
+      <c r="A12" s="86">
+        <v>11</v>
+      </c>
+      <c r="B12" s="73">
+        <v>44089</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" s="78">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="1" customFormat="1">
+      <c r="A13" s="86">
+        <v>12</v>
+      </c>
+      <c r="B13" s="73">
+        <v>44090</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="78">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="1" customFormat="1">
+      <c r="A14" s="86">
+        <v>13</v>
+      </c>
+      <c r="B14" s="73">
+        <v>44091</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" s="78">
+        <v>0.7</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="1" customFormat="1">
+      <c r="A15" s="86">
+        <v>14</v>
+      </c>
+      <c r="B15" s="74">
+        <v>44092</v>
+      </c>
+      <c r="C15" s="85" t="s">
+        <v>154</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" s="77">
+        <v>0.8</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="1" customFormat="1">
+      <c r="A16" s="86">
+        <v>15</v>
+      </c>
+      <c r="B16" s="73">
+        <v>44093</v>
+      </c>
+      <c r="C16" s="84" t="s">
+        <v>154</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" s="78">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="1" customFormat="1">
+      <c r="A17" s="86">
+        <v>16</v>
+      </c>
+      <c r="B17" s="74">
+        <v>44095</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" s="77">
+        <v>0.7</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="1" customFormat="1" ht="28.8">
+      <c r="A18" s="86">
+        <v>17</v>
+      </c>
+      <c r="B18" s="73">
+        <v>44096</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D18" s="75" t="s">
+        <v>161</v>
+      </c>
+      <c r="E18" s="78">
+        <v>0.7</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="1" customFormat="1">
+      <c r="A19" s="86">
+        <v>18</v>
+      </c>
+      <c r="B19" s="73">
+        <v>44097</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E19" s="78">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="D20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="51">
+        <v>44098</v>
+      </c>
+      <c r="C21" s="81" t="s">
+        <v>154</v>
+      </c>
+      <c r="D21" t="s">
+        <v>164</v>
+      </c>
+      <c r="E21" s="80">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="C22" s="9"/>
+      <c r="D22" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="80">
+        <v>0.6</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="82">
+        <v>44099</v>
+      </c>
       <c r="C23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="B24" s="11"/>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="B25" s="12"/>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="13"/>
-      <c r="C26" t="s">
-        <v>9</v>
+        <v>166</v>
+      </c>
+      <c r="D23" t="s">
+        <v>167</v>
+      </c>
+      <c r="E23" s="80">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="D24" t="s">
+        <v>168</v>
+      </c>
+      <c r="E24" s="80">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="D25" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" s="80">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>21</v>
+      </c>
+      <c r="B27" s="82">
+        <v>44102</v>
+      </c>
+      <c r="C27" s="81" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" s="81" t="s">
+        <v>170</v>
+      </c>
+      <c r="E27" s="80">
+        <v>0.5</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2671,8 +3223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2716,16 +3268,16 @@
       <c r="B2" s="19">
         <v>44075</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="55" t="s">
         <v>110</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="62" t="s">
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="4"/>
@@ -2737,16 +3289,16 @@
       <c r="B3" s="19">
         <v>44076</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="57" t="s">
         <v>112</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="F3" s="64" t="s">
+      <c r="F3" s="58" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="4"/>
@@ -2758,16 +3310,16 @@
       <c r="B4" s="19">
         <v>44077</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="57" t="s">
         <v>115</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="56" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="4"/>
@@ -2779,16 +3331,16 @@
       <c r="B5" s="19">
         <v>44078</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="57" t="s">
         <v>117</v>
       </c>
       <c r="E5" s="21">
         <v>0.4</v>
       </c>
-      <c r="F5" s="62" t="s">
+      <c r="F5" s="56" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="4"/>
@@ -2800,16 +3352,16 @@
       <c r="B6" s="19">
         <v>44081</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="57" t="s">
         <v>118</v>
       </c>
       <c r="E6" s="21">
         <v>0.75</v>
       </c>
-      <c r="F6" s="62" t="s">
+      <c r="F6" s="56" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="4"/>
@@ -2821,16 +3373,16 @@
       <c r="B7" s="19">
         <v>44082</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="57" t="s">
         <v>119</v>
       </c>
       <c r="E7" s="21">
         <v>0.85</v>
       </c>
-      <c r="F7" s="62" t="s">
+      <c r="F7" s="56" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="4"/>
@@ -2842,16 +3394,16 @@
       <c r="B8" s="19">
         <v>44083</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="57" t="s">
         <v>120</v>
       </c>
       <c r="E8" s="21">
         <v>1</v>
       </c>
-      <c r="F8" s="64" t="s">
+      <c r="F8" s="58" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="4"/>
@@ -2863,16 +3415,16 @@
       <c r="B9" s="19">
         <v>44084</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="57" t="s">
         <v>121</v>
       </c>
       <c r="E9" s="21">
         <v>1</v>
       </c>
-      <c r="F9" s="62" t="s">
+      <c r="F9" s="56" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="4"/>
@@ -2884,16 +3436,16 @@
       <c r="B10" s="19">
         <v>44085</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="57" t="s">
         <v>122</v>
       </c>
       <c r="E10" s="21">
         <v>0.7</v>
       </c>
-      <c r="F10" s="62" t="s">
+      <c r="F10" s="56" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="4"/>
@@ -2905,16 +3457,16 @@
       <c r="B11" s="19">
         <v>44088</v>
       </c>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="57" t="s">
         <v>122</v>
       </c>
       <c r="E11" s="21">
         <v>0.75</v>
       </c>
-      <c r="F11" s="62" t="s">
+      <c r="F11" s="56" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="4"/>
@@ -2926,16 +3478,16 @@
       <c r="B12" s="19">
         <v>44089</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="57" t="s">
         <v>122</v>
       </c>
       <c r="E12" s="21">
         <v>0.8</v>
       </c>
-      <c r="F12" s="62" t="s">
+      <c r="F12" s="56" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="4"/>
@@ -2947,16 +3499,16 @@
       <c r="B13" s="19">
         <v>44090</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="57" t="s">
         <v>123</v>
       </c>
       <c r="E13" s="21">
         <v>0.85</v>
       </c>
-      <c r="F13" s="62" t="s">
+      <c r="F13" s="56" t="s">
         <v>6</v>
       </c>
       <c r="G13" s="4"/>
@@ -2968,16 +3520,16 @@
       <c r="B14" s="19">
         <v>44091</v>
       </c>
-      <c r="C14" s="61" t="s">
+      <c r="C14" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="D14" s="63" t="s">
+      <c r="D14" s="57" t="s">
         <v>124</v>
       </c>
       <c r="E14" s="21">
         <v>0.95</v>
       </c>
-      <c r="F14" s="62" t="s">
+      <c r="F14" s="56" t="s">
         <v>6</v>
       </c>
       <c r="G14" s="4"/>
@@ -2989,16 +3541,16 @@
       <c r="B15" s="19">
         <v>44092</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="57" t="s">
         <v>125</v>
       </c>
       <c r="E15" s="21">
         <v>1</v>
       </c>
-      <c r="F15" s="65" t="s">
+      <c r="F15" s="59" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="4"/>
@@ -3010,16 +3562,16 @@
       <c r="B16" s="19">
         <v>44095</v>
       </c>
-      <c r="C16" s="61" t="s">
+      <c r="C16" s="55" t="s">
         <v>126</v>
       </c>
-      <c r="D16" s="63" t="s">
+      <c r="D16" s="57" t="s">
         <v>127</v>
       </c>
       <c r="E16" s="21">
         <v>0.6</v>
       </c>
-      <c r="F16" s="66" t="s">
+      <c r="F16" s="60" t="s">
         <v>6</v>
       </c>
       <c r="G16" s="4"/>
@@ -3031,16 +3583,16 @@
       <c r="B17" s="19">
         <v>44096</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="57" t="s">
         <v>129</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="F17" s="66" t="s">
+      <c r="F17" s="60" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="4"/>
@@ -3052,10 +3604,10 @@
       <c r="B18" s="19">
         <v>44097</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="63" t="s">
+      <c r="D18" s="57" t="s">
         <v>131</v>
       </c>
       <c r="E18" s="21">
@@ -3073,16 +3625,16 @@
       <c r="B19" s="19">
         <v>44098</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="D19" s="63" t="s">
+      <c r="D19" s="57" t="s">
         <v>133</v>
       </c>
       <c r="E19" s="21">
         <v>0.35</v>
       </c>
-      <c r="F19" s="66" t="s">
+      <c r="F19" s="60" t="s">
         <v>6</v>
       </c>
       <c r="G19" s="4"/>
@@ -3094,16 +3646,16 @@
       <c r="B20" s="19">
         <v>44099</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="D20" s="63" t="s">
+      <c r="D20" s="57" t="s">
         <v>133</v>
       </c>
       <c r="E20" s="21">
         <v>0.7</v>
       </c>
-      <c r="F20" s="66" t="s">
+      <c r="F20" s="60" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="4"/>
@@ -3112,13 +3664,13 @@
       <c r="A21" s="18">
         <v>20</v>
       </c>
-      <c r="B21" s="67" t="s">
+      <c r="B21" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="D21" s="63" t="s">
+      <c r="D21" s="57" t="s">
         <v>133</v>
       </c>
       <c r="E21" s="21">
@@ -3131,17 +3683,17 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="48"/>
-      <c r="B22" s="68"/>
-      <c r="C22" s="69"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="71"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="65"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="48"/>
-      <c r="B23" s="68"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="71"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="65"/>
     </row>
     <row r="24" spans="1:7">
       <c r="C24" s="46" t="s">
@@ -3525,12 +4077,12 @@
       <c r="B6" s="19">
         <v>44079</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="57"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="68"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7">
@@ -3540,10 +4092,10 @@
       <c r="B7" s="19">
         <v>44080</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="60"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="71"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7">
@@ -3648,12 +4200,12 @@
       <c r="B13" s="19">
         <v>44086</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="57"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="68"/>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7">
@@ -3663,10 +4215,10 @@
       <c r="B14" s="19">
         <v>44087</v>
       </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="60"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="71"/>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7">
@@ -3771,12 +4323,12 @@
       <c r="B20" s="19">
         <v>44093</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="57"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7">
@@ -3786,10 +4338,10 @@
       <c r="B21" s="19">
         <v>44094</v>
       </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="60"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="71"/>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7">

</xml_diff>